<commit_message>
Update spreadsheet headers & add significance
</commit_message>
<xml_diff>
--- a/__digital_preservation_transfer.xlsx
+++ b/__digital_preservation_transfer.xlsx
@@ -21,20 +21,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="334">
   <si>
     <t xml:space="preserve">Required</t>
   </si>
   <si>
+    <t xml:space="preserve">Required (DR_ATTACH), Optional (ITM, DO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional (ITM, DO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required (ITM, DO)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Optional</t>
   </si>
   <si>
-    <t xml:space="preserve">Optional (ITM, DO)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Required (ITM, DO)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Required (DO, DR_ATTACH)</t>
   </si>
   <si>
@@ -296,6 +299,9 @@
     <t xml:space="preserve">turtle</t>
   </si>
   <si>
+    <t xml:space="preserve">memory_of_the_world</t>
+  </si>
+  <si>
     <t xml:space="preserve">snappy the 🐢.jpg</t>
   </si>
   <si>
@@ -408,9 +414,6 @@
   </si>
   <si>
     <t xml:space="preserve">Digital media - Flashdrive/USB/Thumbdrive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">memory_of_the_world</t>
   </si>
   <si>
     <t xml:space="preserve">Master</t>
@@ -1454,11 +1457,11 @@
   </sheetPr>
   <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="60.66"/>
@@ -1481,7 +1484,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="44.84"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1522,10 +1525,10 @@
         <v>2</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>2</v>
@@ -1534,83 +1537,83 @@
         <v>2</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" s="6" t="n">
         <v>30434</v>
@@ -1622,22 +1625,22 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G4" s="6" t="n">
         <v>30434</v>
@@ -1646,30 +1649,30 @@
         <v>31417</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G5" s="6" t="n">
         <v>41169</v>
@@ -1678,30 +1681,30 @@
         <v>44348</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G6" s="6" t="n">
         <v>27771</v>
@@ -1710,30 +1713,30 @@
         <v>30605</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G7" s="6" t="n">
         <v>36779</v>
@@ -1742,30 +1745,30 @@
         <v>38512</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G8" s="6" t="n">
         <v>40745</v>
@@ -1774,30 +1777,30 @@
         <v>41178</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G9" s="6" t="n">
         <v>37210</v>
@@ -1806,30 +1809,30 @@
         <v>38882</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G10" s="6" t="n">
         <v>26146</v>
@@ -1838,30 +1841,30 @@
         <v>26462</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G11" s="6" t="n">
         <v>36260</v>
@@ -1870,30 +1873,30 @@
         <v>36694</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G12" s="6" t="n">
         <v>43538</v>
@@ -1902,30 +1905,30 @@
         <v>44433</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G13" s="6" t="n">
         <v>36260</v>
@@ -1934,30 +1937,30 @@
         <v>36694</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G14" s="6" t="n">
         <v>43538</v>
@@ -1966,30 +1969,30 @@
         <v>44433</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="S14" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G15" s="6" t="n">
         <v>43538</v>
@@ -1998,30 +2001,30 @@
         <v>44433</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="S15" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G16" s="6" t="n">
         <v>43538</v>
@@ -2029,31 +2032,34 @@
       <c r="I16" s="6" t="n">
         <v>44433</v>
       </c>
+      <c r="N16" s="0" t="s">
+        <v>92</v>
+      </c>
       <c r="R16" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S16" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G17" s="6" t="n">
         <v>41169</v>
@@ -2062,10 +2068,10 @@
         <v>44348</v>
       </c>
       <c r="R17" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="S17" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5093,10 +5099,6 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="13">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:B2" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4:B16 B18:B1005" type="list">
       <formula1>INDIRECT("RecordType")</formula1>
       <formula2>0</formula2>
@@ -5145,6 +5147,10 @@
       <formula1>INDIRECT("SensitivityLabel")</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:B2" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5167,7 +5173,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.83"/>
@@ -5182,222 +5188,222 @@
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="I1" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="16" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="0" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F7" s="15"/>
       <c r="I7" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F8" s="15"/>
       <c r="I8" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J8" s="19"/>
     </row>
@@ -5405,10 +5411,10 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F9" s="15"/>
       <c r="J9" s="19"/>
@@ -5417,10 +5423,10 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F10" s="15"/>
       <c r="J10" s="19"/>
@@ -5429,10 +5435,10 @@
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F11" s="15"/>
       <c r="J11" s="19"/>
@@ -5441,10 +5447,10 @@
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F12" s="15"/>
     </row>
@@ -5452,10 +5458,10 @@
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F13" s="15"/>
     </row>
@@ -5463,10 +5469,10 @@
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F14" s="15"/>
     </row>
@@ -5474,10 +5480,10 @@
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F15" s="15"/>
     </row>
@@ -5485,10 +5491,10 @@
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F16" s="15"/>
     </row>
@@ -5496,10 +5502,10 @@
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F17" s="15"/>
     </row>
@@ -5507,10 +5513,10 @@
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F18" s="15"/>
     </row>
@@ -5518,10 +5524,10 @@
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F19" s="15"/>
     </row>
@@ -5529,10 +5535,10 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="16" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F20" s="15"/>
     </row>
@@ -5540,10 +5546,10 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F21" s="15"/>
     </row>
@@ -5551,10 +5557,10 @@
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F22" s="15"/>
     </row>
@@ -5562,10 +5568,10 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F23" s="15"/>
     </row>
@@ -5573,10 +5579,10 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="16" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F24" s="15"/>
     </row>
@@ -5584,10 +5590,10 @@
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F25" s="15"/>
     </row>
@@ -5595,10 +5601,10 @@
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F26" s="15"/>
     </row>
@@ -5606,10 +5612,10 @@
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="16" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F27" s="15"/>
     </row>
@@ -5617,10 +5623,10 @@
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="16" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F28" s="15"/>
     </row>
@@ -5628,10 +5634,10 @@
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="16" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F29" s="15"/>
     </row>
@@ -5639,10 +5645,10 @@
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="17" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F30" s="15"/>
     </row>
@@ -5650,10 +5656,10 @@
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="17" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F31" s="15"/>
     </row>
@@ -5661,10 +5667,10 @@
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="17" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F32" s="15"/>
     </row>
@@ -5672,10 +5678,10 @@
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="17" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F33" s="15"/>
     </row>
@@ -5683,10 +5689,10 @@
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F34" s="15"/>
     </row>
@@ -5694,10 +5700,10 @@
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="17" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F35" s="15"/>
     </row>
@@ -5705,10 +5711,10 @@
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="17" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F36" s="15"/>
     </row>
@@ -5716,10 +5722,10 @@
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F37" s="15"/>
     </row>
@@ -5727,10 +5733,10 @@
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
       <c r="D38" s="17" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F38" s="15"/>
     </row>
@@ -5738,611 +5744,611 @@
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F39" s="15"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="16" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F40" s="15"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D41" s="17" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D42" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D43" s="17" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D45" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D46" s="17" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D47" s="17" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D48" s="17" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D49" s="17" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D50" s="16" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D51" s="16" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D52" s="16" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D53" s="16" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D54" s="16" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D55" s="16" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D56" s="16" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D57" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D58" s="17" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D59" s="17" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D60" s="16" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D61" s="17" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D62" s="17" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D63" s="17" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D64" s="17" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D65" s="17" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D66" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D67" s="17" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D68" s="17" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D69" s="17" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D70" s="16" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D71" s="17" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D72" s="17" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D73" s="17" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D74" s="17" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D75" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D76" s="17" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D77" s="16" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D78" s="17" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D79" s="17" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D80" s="17" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D81" s="17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D82" s="17" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D83" s="17" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D84" s="17" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D85" s="17" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D86" s="17" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D87" s="17" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D88" s="17" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D89" s="17" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D90" s="17" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D91" s="17" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D92" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D93" s="17" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D94" s="17" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D95" s="17" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D96" s="17" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D97" s="17" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D98" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D99" s="17" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D100" s="17" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D101" s="17" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D102" s="17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D103" s="17" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D104" s="16" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D105" s="17" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D106" s="17" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D107" s="17" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D108" s="17" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D109" s="17" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D110" s="17" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D111" s="17" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D112" s="17" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D113" s="17" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D114" s="17" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D115" s="17" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D116" s="17" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D117" s="17" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D118" s="17" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D119" s="17" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D120" s="17" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D121" s="17" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D122" s="17" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D123" s="17" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D124" s="17" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D125" s="17" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D126" s="17" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D127" s="17" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D128" s="17" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D129" s="23" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D130" s="20" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D131" s="20" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D132" s="16" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D133" s="17" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D134" s="17" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D135" s="17" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D136" s="17" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D137" s="17" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D138" s="17" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D139" s="17" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D140" s="16" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D141" s="16" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D142" s="16" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D143" s="16" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D144" s="16" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D145" s="16" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D146" s="16" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D147" s="16" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D148" s="16" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D149" s="16" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D150" s="16" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D151" s="16" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Don't inherit the significance
</commit_message>
<xml_diff>
--- a/__digital_preservation_transfer.xlsx
+++ b/__digital_preservation_transfer.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="334">
   <si>
     <t xml:space="preserve">Required</t>
   </si>
@@ -302,6 +302,9 @@
     <t xml:space="preserve">memory_of_the_world</t>
   </si>
   <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">snappy the 🐢.jpg</t>
   </si>
   <si>
@@ -339,9 +342,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
   </si>
   <si>
     <t xml:space="preserve">approximate</t>
@@ -1458,10 +1458,10 @@
   <dimension ref="A1:S1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
+      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="60.66"/>
@@ -2035,11 +2035,14 @@
       <c r="N16" s="0" t="s">
         <v>92</v>
       </c>
+      <c r="O16" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="R16" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S16" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2068,7 +2071,7 @@
         <v>44348</v>
       </c>
       <c r="R17" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S17" s="0" t="s">
         <v>40</v>
@@ -5173,7 +5176,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.83"/>
@@ -5188,19 +5191,19 @@
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>21</v>
@@ -5212,16 +5215,16 @@
         <v>18</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5229,25 +5232,25 @@
         <v>26</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -5255,7 +5258,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>107</v>

</xml_diff>